<commit_message>
organize code; create connection matrix to innermodel; adapt code to connection matrix; some bug fixes;
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\DESCRIPTIVE I\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\DA_PSM_NEW\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
   <si>
     <t xml:space="preserve">SOURCE </t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>VALUE</t>
+  </si>
+  <si>
+    <t>FROM</t>
+  </si>
+  <si>
+    <t>TO</t>
   </si>
 </sst>
 </file>
@@ -691,10 +697,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C1" sqref="C1:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,162 +708,92 @@
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
       <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>28</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -869,7 +805,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{869AC768-4351-4488-BEC4-3815B6879419}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9431A7EE-D921-4140-B8BE-F61E264E316E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/PowerBIAddIn"/>
   </ds:schemaRefs>

</xml_diff>